<commit_message>
Fix date in Plantain observed data (less then a day difference in measurements)
</commit_message>
<xml_diff>
--- a/Tests/Validation/Plantain/Observed.xlsx
+++ b/Tests/Validation/Plantain/Observed.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ApsimX\Prototypes\Plantain\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ApsimX\Tests\Validation\Plantain\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,6 +15,9 @@
     <sheet name="Notes" sheetId="13" r:id="rId1"/>
     <sheet name="Observed" sheetId="16" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Observed!$A$1:$AK$1519</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -38,7 +41,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Cichota, Rogerio:</t>
         </r>
@@ -47,7 +50,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Average of treatment</t>
@@ -62,7 +65,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Cichota, Rogerio:</t>
         </r>
@@ -71,7 +74,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Using average of treatment</t>
@@ -86,7 +89,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Cichota, Rogerio:</t>
         </r>
@@ -95,7 +98,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Using average of treatment</t>
@@ -110,7 +113,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Cichota, Rogerio:</t>
         </r>
@@ -119,7 +122,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Using average of treatment</t>
@@ -134,7 +137,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Cichota, Rogerio:</t>
         </r>
@@ -143,7 +146,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Using average of treatment</t>
@@ -530,14 +533,14 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1012,10 +1015,10 @@
   <dimension ref="A1:AK1519"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="F1056" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E4" sqref="E4"/>
+      <selection pane="bottomRight" activeCell="C1063" sqref="C1063"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -47947,7 +47950,7 @@
         <v>55</v>
       </c>
       <c r="C1056" s="9">
-        <v>42304</v>
+        <v>42303</v>
       </c>
       <c r="D1056" t="s">
         <v>66</v>
@@ -47980,7 +47983,7 @@
         <v>55</v>
       </c>
       <c r="C1057" s="9">
-        <v>42304</v>
+        <v>42303</v>
       </c>
       <c r="D1057" t="s">
         <v>66</v>
@@ -48013,7 +48016,7 @@
         <v>55</v>
       </c>
       <c r="C1058" s="9">
-        <v>42304</v>
+        <v>42303</v>
       </c>
       <c r="D1058" t="s">
         <v>66</v>
@@ -48046,7 +48049,7 @@
         <v>55</v>
       </c>
       <c r="C1059" s="9">
-        <v>42304</v>
+        <v>42303</v>
       </c>
       <c r="D1059" t="s">
         <v>66</v>
@@ -48079,7 +48082,7 @@
         <v>55</v>
       </c>
       <c r="C1060" s="9">
-        <v>42304</v>
+        <v>42303</v>
       </c>
       <c r="D1060" t="s">
         <v>66</v>
@@ -48112,7 +48115,7 @@
         <v>55</v>
       </c>
       <c r="C1061" s="9">
-        <v>42304</v>
+        <v>42303</v>
       </c>
       <c r="D1061" t="s">
         <v>66</v>
@@ -48145,7 +48148,7 @@
         <v>55</v>
       </c>
       <c r="C1062" s="9">
-        <v>42304</v>
+        <v>42303</v>
       </c>
       <c r="D1062" t="s">
         <v>66</v>
@@ -48178,7 +48181,7 @@
         <v>55</v>
       </c>
       <c r="C1063" s="9">
-        <v>42304</v>
+        <v>42303</v>
       </c>
       <c r="D1063" t="s">
         <v>66</v>
@@ -48211,7 +48214,7 @@
         <v>55</v>
       </c>
       <c r="C1064" s="9">
-        <v>42304</v>
+        <v>42303</v>
       </c>
       <c r="D1064" t="s">
         <v>66</v>
@@ -48244,7 +48247,7 @@
         <v>55</v>
       </c>
       <c r="C1065" s="9">
-        <v>42304</v>
+        <v>42303</v>
       </c>
       <c r="D1065" t="s">
         <v>66</v>
@@ -48277,7 +48280,7 @@
         <v>55</v>
       </c>
       <c r="C1066" s="9">
-        <v>42304</v>
+        <v>42303</v>
       </c>
       <c r="D1066" t="s">
         <v>66</v>
@@ -48310,7 +48313,7 @@
         <v>55</v>
       </c>
       <c r="C1067" s="9">
-        <v>42304</v>
+        <v>42303</v>
       </c>
       <c r="D1067" t="s">
         <v>66</v>
@@ -48343,7 +48346,7 @@
         <v>55</v>
       </c>
       <c r="C1068" s="9">
-        <v>42304</v>
+        <v>42303</v>
       </c>
       <c r="D1068" t="s">
         <v>66</v>
@@ -48376,7 +48379,7 @@
         <v>55</v>
       </c>
       <c r="C1069" s="9">
-        <v>42304</v>
+        <v>42303</v>
       </c>
       <c r="D1069" t="s">
         <v>66</v>
@@ -48409,7 +48412,7 @@
         <v>55</v>
       </c>
       <c r="C1070" s="9">
-        <v>42304</v>
+        <v>42303</v>
       </c>
       <c r="D1070" t="s">
         <v>66</v>
@@ -48442,7 +48445,7 @@
         <v>55</v>
       </c>
       <c r="C1071" s="9">
-        <v>42304</v>
+        <v>42303</v>
       </c>
       <c r="D1071" t="s">
         <v>66</v>
@@ -48475,7 +48478,7 @@
         <v>55</v>
       </c>
       <c r="C1072" s="9">
-        <v>42304</v>
+        <v>42303</v>
       </c>
       <c r="D1072" t="s">
         <v>66</v>
@@ -48508,7 +48511,7 @@
         <v>55</v>
       </c>
       <c r="C1073" s="9">
-        <v>42304</v>
+        <v>42303</v>
       </c>
       <c r="D1073" t="s">
         <v>66</v>

</xml_diff>